<commit_message>
fix typo and groupbox height
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/autoFill.xlsx
+++ b/src/main/webapp/WEB-INF/books/autoFill.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/zssessentials/src/main/webapp/WEB-INF/books/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0103D974-CA47-BC4A-A7B0-602B7C156E02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45380" yWindow="4220" windowWidth="17040" windowHeight="11280"/>
+    <workbookView xWindow="45380" yWindow="4220" windowWidth="17040" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Auto Fill Sample 1</t>
   </si>
@@ -65,16 +66,19 @@
     <t>Week day - short</t>
   </si>
   <si>
-    <t>Janurary</t>
-  </si>
-  <si>
     <t>Mon</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>select B8:B14 and drag</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -96,6 +100,7 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -167,6 +172,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -458,11 +466,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -487,6 +495,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
@@ -516,7 +529,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.2">
@@ -524,7 +537,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.2">

</xml_diff>